<commit_message>
changes after RI looked at code
</commit_message>
<xml_diff>
--- a/Data/Discussion/Complexity/Regulations_analysis_words.xlsx
+++ b/Data/Discussion/Complexity/Regulations_analysis_words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fa24575\Dropbox\Organic Waste Bans\06. Post SYP\03.2.Complexity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C33EAC7-5D1A-4986-919D-DFC524F394B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7E35AA-52A4-4EC9-BC4C-7D11173206E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21150" activeTab="1" xr2:uid="{7C6E7C5E-D305-473D-BC78-E5030630A3AC}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{7C6E7C5E-D305-473D-BC78-E5030630A3AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1836,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0727893A-A29B-415C-94F5-65F51CAB0D53}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,8 +2047,8 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <f>5+4+10+15+18+5+5+5</f>
-        <v>67</v>
+        <f>5+4+4+4+10+15+18+5+5+5</f>
+        <v>75</v>
       </c>
       <c r="C9">
         <f>4+4+5+5+5+5+5+5+5+9+20</f>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="F9" s="1">
         <f>SUM(B9:C9)</f>
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="G9" s="1">
         <f>2+E9</f>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="C42">
         <f t="shared" si="8"/>
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D42">
         <f t="shared" si="7"/>
@@ -2597,7 +2597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3C8F8B-8244-468F-8A9A-A6F447C263B9}">
   <dimension ref="A1:H179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>